<commit_message>
agregado del filtro por categorias
</commit_message>
<xml_diff>
--- a/redes/listado de artistas.xlsx
+++ b/redes/listado de artistas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Expo permanente" sheetId="1" r:id="rId1"/>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +935,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1422,7 +1422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1645,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,7 +1679,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1734,7 +1734,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1744,8 +1744,8 @@
         <v>19</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1756,7 +1756,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1766,8 +1766,8 @@
         <v>27</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1799,8 +1799,8 @@
         <v>35</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1844,7 +1844,7 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1877,7 +1877,7 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1908,9 +1908,9 @@
       <c r="B23" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="E24" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1947,5 +1947,6 @@
     <hyperlink ref="B22" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
arreglo de la ruta de rosario amendolara, cata gonsalez, vanessa rojas, pablo delbene y andres amaya para el funcionamiento del boton de mostrar un artista aleatorio
</commit_message>
<xml_diff>
--- a/redes/listado de artistas.xlsx
+++ b/redes/listado de artistas.xlsx
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1015,7 +1015,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">

</xml_diff>

<commit_message>
actualizacion de la nueva muestra y agregado de artistas
</commit_message>
<xml_diff>
--- a/redes/listado de artistas.xlsx
+++ b/redes/listado de artistas.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="116">
   <si>
     <t>NOMBRE DEL ARTISTA</t>
   </si>
@@ -106,9 +106,6 @@
     <t>https://www.instagram.com/pablofunes/</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>https://www.instagram.com/ramen.art/</t>
   </si>
   <si>
@@ -199,24 +196,9 @@
     <t>eva.ferran</t>
   </si>
   <si>
-    <t>el_arte_.descalzo</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/el_arte_.descalzo/</t>
-  </si>
-  <si>
     <t>https://www.instagram.com/male.bianco5/</t>
   </si>
   <si>
-    <t>esperar</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/medioacida/</t>
-  </si>
-  <si>
-    <t>medioacida</t>
-  </si>
-  <si>
     <t>https://www.instagram.com/feli.paez/</t>
   </si>
   <si>
@@ -229,12 +211,6 @@
     <t>https://www.instagram.com/moroarielfernando/</t>
   </si>
   <si>
-    <t>etamenendez</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/etamenendez/</t>
-  </si>
-  <si>
     <t>kvhlilk90s</t>
   </si>
   <si>
@@ -253,18 +229,6 @@
     <t>foto-video</t>
   </si>
   <si>
-    <t>textos</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/inairammartin/</t>
-  </si>
-  <si>
-    <t>inairammartin</t>
-  </si>
-  <si>
-    <t>escultura</t>
-  </si>
-  <si>
     <t>MES</t>
   </si>
   <si>
@@ -313,9 +277,6 @@
     <t>beluu.abdala</t>
   </si>
   <si>
-    <t>EN ESPERA</t>
-  </si>
-  <si>
     <t>JUNIO</t>
   </si>
   <si>
@@ -337,23 +298,89 @@
     <t>micreorelatos</t>
   </si>
   <si>
-    <t>CONSULTADO</t>
-  </si>
-  <si>
-    <t>SI-NO</t>
-  </si>
-  <si>
     <t>EN PAGINA</t>
   </si>
   <si>
-    <t>https://www.instagram.com/beluu.abdala/</t>
+    <t xml:space="preserve">OCTUBRE NO </t>
+  </si>
+  <si>
+    <t>NOVIEMBRE</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/fiorelladibujando/</t>
+  </si>
+  <si>
+    <t>fiorelladibujando</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/gabb.lobato/</t>
+  </si>
+  <si>
+    <t>gabb.lobato</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/jimenaramos_y/</t>
+  </si>
+  <si>
+    <t>jimenaramos_y</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/lerolera_/</t>
+  </si>
+  <si>
+    <t>lerolera_</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/vanessa.karin_/</t>
+  </si>
+  <si>
+    <t>vanessa.karin_</t>
+  </si>
+  <si>
+    <t>ilustracion-animacion</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/claudiaperezturk/</t>
+  </si>
+  <si>
+    <t>claudiaperezturk</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/tania_sagle/</t>
+  </si>
+  <si>
+    <t>tania_sagle</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/lagaleriadeserge/</t>
+  </si>
+  <si>
+    <t>lagaleriadeserge</t>
+  </si>
+  <si>
+    <t>DICIEMBRE</t>
+  </si>
+  <si>
+    <t>smont_herz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">animacion </t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/muni.foto/</t>
+  </si>
+  <si>
+    <t>muni.foto</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/smont_herz/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,22 +421,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -420,6 +431,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -490,7 +509,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
@@ -498,10 +517,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
@@ -786,18 +804,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:H13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -820,18 +837,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -843,10 +860,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>17</v>
@@ -907,13 +924,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -955,10 +972,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -971,13 +988,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -987,10 +1004,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
@@ -998,15 +1015,15 @@
       <c r="D12" s="3"/>
       <c r="E12" s="5"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="9"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
@@ -1019,26 +1036,26 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
@@ -1061,7 +1078,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1073,10 +1090,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>21</v>
@@ -1085,17 +1102,17 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1111,7 +1128,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1121,13 +1138,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1163,7 +1180,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1175,66 +1192,66 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1248,7 +1265,9 @@
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1268,7 +1287,9 @@
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1277,126 +1298,367 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>61</v>
+        <v>102</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="D37" s="3"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>68</v>
+        <v>105</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>76</v>
+        <v>107</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="D39" s="3"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
       <c r="H41" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F46" s="8"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1410,11 +1672,16 @@
     <hyperlink ref="B5" r:id="rId8"/>
     <hyperlink ref="B18" r:id="rId9"/>
     <hyperlink ref="B28" r:id="rId10"/>
-    <hyperlink ref="B40" r:id="rId11"/>
-    <hyperlink ref="B27" r:id="rId12"/>
+    <hyperlink ref="B27" r:id="rId11"/>
+    <hyperlink ref="B35" r:id="rId12"/>
+    <hyperlink ref="B36" r:id="rId13"/>
+    <hyperlink ref="B37" r:id="rId14"/>
+    <hyperlink ref="B38" r:id="rId15"/>
+    <hyperlink ref="B39" r:id="rId16"/>
+    <hyperlink ref="B40" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -1423,7 +1690,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,84 +1702,84 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>59</v>
+        <v>76</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1643,10 +1910,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:E23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,296 +1924,167 @@
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B5" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B12" r:id="rId9"/>
-    <hyperlink ref="B14" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="B15" r:id="rId12"/>
-    <hyperlink ref="B20" r:id="rId13"/>
-    <hyperlink ref="B17" r:id="rId14" display="https://www.instagram.com/artedanielolcay/"/>
-    <hyperlink ref="B16" r:id="rId15" display="https://www.instagram.com/bladeva_digital/"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.instagram.com/kvhlilk90s/"/>
-    <hyperlink ref="B24" r:id="rId17"/>
-    <hyperlink ref="B23" r:id="rId18"/>
-    <hyperlink ref="B21" r:id="rId19"/>
-    <hyperlink ref="B22" r:id="rId20"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="B3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregado de pablo puenta al shop
</commit_message>
<xml_diff>
--- a/redes/listado de artistas.xlsx
+++ b/redes/listado de artistas.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="131">
   <si>
     <t>NOMBRE DEL ARTISTA</t>
   </si>
@@ -55,12 +55,6 @@
     <t>fotografía</t>
   </si>
   <si>
-    <t>pah.del</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/pah.del/</t>
-  </si>
-  <si>
     <t>ilustración-video</t>
   </si>
   <si>
@@ -415,14 +409,23 @@
     <t>ilustracion digital</t>
   </si>
   <si>
-    <t>falta la permanente</t>
+    <t>https://www.instagram.com/pablo_delbene/</t>
+  </si>
+  <si>
+    <t>pablo_delbene</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/fernanda.gese/</t>
+  </si>
+  <si>
+    <t>fernanda.gese</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,13 +436,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -485,16 +481,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,11 +492,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -552,32 +535,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
-    <cellStyle name="Hipervínculo" xfId="4" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Salida" xfId="3" builtinId="21"/>
+    <cellStyle name="Salida" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -857,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,18 +867,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -911,226 +890,230 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1141,98 +1124,98 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1243,82 +1226,82 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>54</v>
+        <v>62</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
+        <v>64</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1328,7 +1311,9 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1338,9 +1323,7 @@
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1351,162 +1334,162 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="8"/>
+        <v>110</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="1"/>
+        <v>101</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1517,110 +1500,110 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="2"/>
+        <v>108</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G45" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>124</v>
+        <v>114</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>119</v>
+        <v>123</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1727,29 +1710,30 @@
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B22" r:id="rId3"/>
-    <hyperlink ref="B19" r:id="rId4"/>
+    <hyperlink ref="B23" r:id="rId3"/>
+    <hyperlink ref="B20" r:id="rId4"/>
     <hyperlink ref="B3" r:id="rId5"/>
     <hyperlink ref="B7" r:id="rId6"/>
     <hyperlink ref="B6" r:id="rId7"/>
     <hyperlink ref="B5" r:id="rId8"/>
-    <hyperlink ref="B18" r:id="rId9"/>
-    <hyperlink ref="B28" r:id="rId10"/>
-    <hyperlink ref="B27" r:id="rId11"/>
-    <hyperlink ref="B35" r:id="rId12"/>
-    <hyperlink ref="B36" r:id="rId13"/>
-    <hyperlink ref="B37" r:id="rId14"/>
-    <hyperlink ref="B38" r:id="rId15"/>
-    <hyperlink ref="B39" r:id="rId16"/>
-    <hyperlink ref="B40" r:id="rId17"/>
-    <hyperlink ref="B44" r:id="rId18"/>
-    <hyperlink ref="B48" r:id="rId19"/>
-    <hyperlink ref="B46" r:id="rId20"/>
-    <hyperlink ref="B49" r:id="rId21"/>
-    <hyperlink ref="B47" r:id="rId22"/>
+    <hyperlink ref="B19" r:id="rId9"/>
+    <hyperlink ref="B29" r:id="rId10"/>
+    <hyperlink ref="B28" r:id="rId11"/>
+    <hyperlink ref="B36" r:id="rId12"/>
+    <hyperlink ref="B37" r:id="rId13"/>
+    <hyperlink ref="B38" r:id="rId14"/>
+    <hyperlink ref="B39" r:id="rId15"/>
+    <hyperlink ref="B40" r:id="rId16"/>
+    <hyperlink ref="B41" r:id="rId17"/>
+    <hyperlink ref="B45" r:id="rId18"/>
+    <hyperlink ref="B49" r:id="rId19"/>
+    <hyperlink ref="B47" r:id="rId20"/>
+    <hyperlink ref="B50" r:id="rId21"/>
+    <hyperlink ref="B48" r:id="rId22"/>
+    <hyperlink ref="B16" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 
@@ -1770,98 +1754,98 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>56</v>
+        <v>74</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2008,63 +1992,63 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
correccion de la foto de fiore y de las obras de ariel moro en shop
</commit_message>
<xml_diff>
--- a/redes/listado de artistas.xlsx
+++ b/redes/listado de artistas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Expo permanente" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="152">
   <si>
     <t>NOMBRE DEL ARTISTA</t>
   </si>
@@ -419,13 +419,76 @@
   </si>
   <si>
     <t>fernanda.gese</t>
+  </si>
+  <si>
+    <t>ENERO VACACIONES</t>
+  </si>
+  <si>
+    <t>FEBRERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enero </t>
+  </si>
+  <si>
+    <t>VACACIONES</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/yoel_acost/</t>
+  </si>
+  <si>
+    <t>yoel_acost</t>
+  </si>
+  <si>
+    <t>fotografia - video</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/limerencia212/</t>
+  </si>
+  <si>
+    <t>limerencia212</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/juliusandfriendz/</t>
+  </si>
+  <si>
+    <t>juliusandfriendz</t>
+  </si>
+  <si>
+    <t>video  - poemas</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/by.ornebad/</t>
+  </si>
+  <si>
+    <t>by.ornebad</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/carolina.quiroga.blanco/</t>
+  </si>
+  <si>
+    <t>carolina.quiroga.blanco</t>
+  </si>
+  <si>
+    <t>collage</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/sangarufa/</t>
+  </si>
+  <si>
+    <t>ilustraciones</t>
+  </si>
+  <si>
+    <t>sangarufa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,8 +544,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -497,6 +567,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -535,13 +610,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
@@ -551,10 +627,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="4" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="4" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Salida" xfId="2" builtinId="21"/>
   </cellStyles>
@@ -836,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1188,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="7"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -1358,7 +1436,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="1"/>
+      <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -1374,7 +1452,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="1"/>
+      <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -1617,7 +1695,9 @@
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1637,7 +1717,9 @@
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1647,53 +1729,81 @@
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="A57" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
       <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
+      <c r="A59" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -1731,9 +1841,13 @@
     <hyperlink ref="B50" r:id="rId21"/>
     <hyperlink ref="B48" r:id="rId22"/>
     <hyperlink ref="B16" r:id="rId23"/>
+    <hyperlink ref="B56" r:id="rId24"/>
+    <hyperlink ref="B57" r:id="rId25"/>
+    <hyperlink ref="B58" r:id="rId26"/>
+    <hyperlink ref="B59" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
 
@@ -1741,8 +1855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1849,16 +1963,28 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -1963,8 +2089,11 @@
       <c r="D26" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
modificacion de rutas para la finalizacion del proyecto
</commit_message>
<xml_diff>
--- a/redes/listado de artistas.xlsx
+++ b/redes/listado de artistas.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="160">
   <si>
     <t>NOMBRE DEL ARTISTA</t>
   </si>
@@ -485,6 +485,27 @@
   </si>
   <si>
     <t>zaelvonmazon</t>
+  </si>
+  <si>
+    <t>MARZO</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/by.ornebad/</t>
+  </si>
+  <si>
+    <t>by.ornebad</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/jai._17/</t>
+  </si>
+  <si>
+    <t>jai._17</t>
+  </si>
+  <si>
+    <t>AGREGAR PORFOLIO DE FERNANDA GESE</t>
+  </si>
+  <si>
+    <t>faltan textos</t>
   </si>
 </sst>
 </file>
@@ -918,7 +939,7 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,7 +1492,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="1"/>
+      <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -1535,7 +1556,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="1"/>
+      <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -1822,8 +1843,12 @@
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -1832,23 +1857,37 @@
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
+      <c r="A62" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+      <c r="A63" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -1920,9 +1959,11 @@
     <hyperlink ref="B57" r:id="rId25"/>
     <hyperlink ref="B58" r:id="rId26"/>
     <hyperlink ref="B59" r:id="rId27"/>
+    <hyperlink ref="B62" r:id="rId28"/>
+    <hyperlink ref="B63" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 

</xml_diff>